<commit_message>
NLP & WordCloud 1.1
</commit_message>
<xml_diff>
--- a/data/word_frequency.xlsx
+++ b/data/word_frequency.xlsx
@@ -25,12 +25,6 @@
     <t>吃</t>
   </si>
   <si>
-    <t>叔</t>
-  </si>
-  <si>
-    <t>五郎</t>
-  </si>
-  <si>
     <t>吃饭</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>大叔</t>
   </si>
   <si>
-    <t>季</t>
-  </si>
-  <si>
     <t>最后</t>
   </si>
   <si>
@@ -104,9 +95,6 @@
     <t>觉得</t>
   </si>
   <si>
-    <t>没有</t>
-  </si>
-  <si>
     <t>孤独</t>
   </si>
   <si>
@@ -119,99 +107,90 @@
     <t>饭</t>
   </si>
   <si>
+    <t>更</t>
+  </si>
+  <si>
+    <t>每次</t>
+  </si>
+  <si>
     <t>哈哈哈</t>
   </si>
   <si>
-    <t>每次</t>
-  </si>
-  <si>
-    <t>更</t>
-  </si>
-  <si>
     <t>可爱</t>
   </si>
   <si>
+    <t>生活</t>
+  </si>
+  <si>
     <t>日本</t>
   </si>
   <si>
-    <t>生活</t>
-  </si>
-  <si>
     <t>里</t>
   </si>
   <si>
     <t>烤肉</t>
   </si>
   <si>
+    <t>香</t>
+  </si>
+  <si>
+    <t>口罩</t>
+  </si>
+  <si>
     <t>疫情</t>
   </si>
   <si>
-    <t>口罩</t>
-  </si>
-  <si>
-    <t>香</t>
-  </si>
-  <si>
     <t>集</t>
   </si>
   <si>
-    <t>（</t>
-  </si>
-  <si>
     <t>没</t>
   </si>
   <si>
+    <t>饿</t>
+  </si>
+  <si>
+    <t>这种</t>
+  </si>
+  <si>
     <t>本季</t>
   </si>
   <si>
-    <t>这种</t>
-  </si>
-  <si>
-    <t>饿</t>
-  </si>
-  <si>
     <t>说</t>
   </si>
   <si>
     <t>看到</t>
   </si>
   <si>
-    <t>已经</t>
+    <t>有点</t>
   </si>
   <si>
     <t>胃口</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>有点</t>
+    <t>享受</t>
+  </si>
+  <si>
+    <t>爱</t>
+  </si>
+  <si>
+    <t>食欲</t>
+  </si>
+  <si>
+    <t>这季</t>
+  </si>
+  <si>
+    <t>真是</t>
+  </si>
+  <si>
+    <t>现在</t>
   </si>
   <si>
     <t>美食家</t>
   </si>
   <si>
-    <t>享受</t>
-  </si>
-  <si>
-    <t>这季</t>
-  </si>
-  <si>
-    <t>爱</t>
-  </si>
-  <si>
-    <t>食欲</t>
-  </si>
-  <si>
     <t>其实</t>
   </si>
   <si>
-    <t>现在</t>
-  </si>
-  <si>
-    <t>真是</t>
-  </si>
-  <si>
     <t>神剧</t>
   </si>
   <si>
@@ -221,706 +200,727 @@
     <t>料理</t>
   </si>
   <si>
+    <t>剧情</t>
+  </si>
+  <si>
     <t>好看</t>
   </si>
   <si>
-    <t>剧情</t>
+    <t>菜</t>
+  </si>
+  <si>
+    <t>特别</t>
   </si>
   <si>
     <t>快乐</t>
   </si>
   <si>
-    <t>特别</t>
-  </si>
-  <si>
-    <t>菜</t>
-  </si>
-  <si>
     <t>陪</t>
   </si>
   <si>
+    <t>馋</t>
+  </si>
+  <si>
     <t>一直</t>
   </si>
   <si>
+    <t>甜点</t>
+  </si>
+  <si>
     <t>希望</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>甜点</t>
-  </si>
-  <si>
-    <t>馋</t>
+    <t>一种</t>
+  </si>
+  <si>
+    <t>中</t>
+  </si>
+  <si>
+    <t>挺</t>
   </si>
   <si>
     <t>时间</t>
   </si>
   <si>
-    <t>挺</t>
-  </si>
-  <si>
-    <t>一种</t>
+    <t>第一季</t>
   </si>
   <si>
     <t>前</t>
   </si>
   <si>
-    <t>中</t>
-  </si>
-  <si>
-    <t>）</t>
-  </si>
-  <si>
-    <t>第一季</t>
+    <t>店</t>
+  </si>
+  <si>
+    <t>不错</t>
+  </si>
+  <si>
+    <t>每集</t>
+  </si>
+  <si>
+    <t>话</t>
+  </si>
+  <si>
+    <t>一如既往</t>
+  </si>
+  <si>
+    <t>继续</t>
   </si>
   <si>
     <t>哈哈</t>
   </si>
   <si>
-    <t>不错</t>
-  </si>
-  <si>
-    <t>继续</t>
-  </si>
-  <si>
-    <t>一如既往</t>
-  </si>
-  <si>
-    <t>店</t>
-  </si>
-  <si>
-    <t>话</t>
-  </si>
-  <si>
-    <t>每集</t>
+    <t>开心</t>
+  </si>
+  <si>
+    <t>十年</t>
   </si>
   <si>
     <t>期待</t>
   </si>
   <si>
+    <t>探店</t>
+  </si>
+  <si>
+    <t>很多</t>
+  </si>
+  <si>
+    <t>有趣</t>
+  </si>
+  <si>
     <t>好多</t>
   </si>
   <si>
-    <t>探店</t>
-  </si>
-  <si>
-    <t>十年</t>
-  </si>
-  <si>
-    <t>开心</t>
-  </si>
-  <si>
-    <t>有趣</t>
-  </si>
-  <si>
-    <t>很多</t>
+    <t>戴</t>
+  </si>
+  <si>
+    <t>哈哈哈哈</t>
   </si>
   <si>
     <t>一年</t>
   </si>
   <si>
-    <t>戴</t>
-  </si>
-  <si>
-    <t>哈哈哈哈</t>
+    <t>度过</t>
   </si>
   <si>
     <t>知道</t>
   </si>
   <si>
-    <t>度过</t>
+    <t>越来越</t>
+  </si>
+  <si>
+    <t>时</t>
+  </si>
+  <si>
+    <t>时光</t>
+  </si>
+  <si>
+    <t>永远</t>
+  </si>
+  <si>
+    <t>发现</t>
+  </si>
+  <si>
+    <t>比较</t>
+  </si>
+  <si>
+    <t>真</t>
   </si>
   <si>
     <t>做</t>
   </si>
   <si>
-    <t>时</t>
-  </si>
-  <si>
-    <t>时光</t>
-  </si>
-  <si>
     <t>烤</t>
   </si>
   <si>
-    <t>永远</t>
+    <t>这部</t>
+  </si>
+  <si>
+    <t>第十</t>
   </si>
   <si>
     <t>出</t>
   </si>
   <si>
-    <t>这部</t>
-  </si>
-  <si>
-    <t>比较</t>
-  </si>
-  <si>
-    <t>真</t>
-  </si>
-  <si>
-    <t>系列</t>
-  </si>
-  <si>
-    <t>!</t>
-  </si>
-  <si>
-    <t>发现</t>
-  </si>
-  <si>
-    <t>第十</t>
-  </si>
-  <si>
-    <t>越来越</t>
+    <t>感谢</t>
+  </si>
+  <si>
+    <t>一起</t>
+  </si>
+  <si>
+    <t>那集</t>
+  </si>
+  <si>
+    <t>找</t>
+  </si>
+  <si>
+    <t>台湾</t>
+  </si>
+  <si>
+    <t>时期</t>
+  </si>
+  <si>
+    <t>表情</t>
+  </si>
+  <si>
+    <t>深夜</t>
   </si>
   <si>
     <t>猪排</t>
   </si>
   <si>
-    <t>台湾</t>
-  </si>
-  <si>
-    <t>表情</t>
-  </si>
-  <si>
-    <t>时期</t>
-  </si>
-  <si>
     <t>完全</t>
   </si>
   <si>
-    <t>感谢</t>
-  </si>
-  <si>
-    <t>深夜</t>
-  </si>
-  <si>
     <t>终于</t>
   </si>
   <si>
-    <t>找</t>
-  </si>
-  <si>
-    <t>那集</t>
-  </si>
-  <si>
-    <t>一起</t>
+    <t>作者</t>
+  </si>
+  <si>
+    <t>一天</t>
+  </si>
+  <si>
+    <t>味道</t>
+  </si>
+  <si>
+    <t>盖饭</t>
+  </si>
+  <si>
+    <t>以前</t>
+  </si>
+  <si>
+    <t>工作</t>
+  </si>
+  <si>
+    <t>猪肉</t>
+  </si>
+  <si>
+    <t>第二季</t>
+  </si>
+  <si>
+    <t>肉</t>
+  </si>
+  <si>
+    <t>陪伴</t>
+  </si>
+  <si>
+    <t>每天</t>
   </si>
   <si>
     <t>好像</t>
   </si>
   <si>
+    <t>印象</t>
+  </si>
+  <si>
+    <t>站</t>
+  </si>
+  <si>
     <t>菠萝</t>
   </si>
   <si>
-    <t>每天</t>
-  </si>
-  <si>
-    <t>味道</t>
-  </si>
-  <si>
-    <t>肉</t>
-  </si>
-  <si>
-    <t>第二季</t>
-  </si>
-  <si>
-    <t>以前</t>
-  </si>
-  <si>
-    <t>站</t>
-  </si>
-  <si>
-    <t>工作</t>
-  </si>
-  <si>
-    <t>一天</t>
-  </si>
-  <si>
-    <t>作者</t>
-  </si>
-  <si>
-    <t>印象</t>
-  </si>
-  <si>
-    <t>猪肉</t>
-  </si>
-  <si>
-    <t>陪伴</t>
-  </si>
-  <si>
-    <t>盖饭</t>
+    <t>世界</t>
+  </si>
+  <si>
+    <t>心情</t>
+  </si>
+  <si>
+    <t>看起来</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>一下</t>
+  </si>
+  <si>
+    <t>标记</t>
+  </si>
+  <si>
+    <t>点</t>
+  </si>
+  <si>
+    <t>特殊</t>
+  </si>
+  <si>
+    <t>年</t>
+  </si>
+  <si>
+    <t>吸引</t>
+  </si>
+  <si>
+    <t>最近</t>
+  </si>
+  <si>
+    <t>不会</t>
+  </si>
+  <si>
+    <t>人生</t>
+  </si>
+  <si>
+    <t>镜头</t>
+  </si>
+  <si>
+    <t>内心</t>
   </si>
   <si>
     <t>满足</t>
   </si>
   <si>
-    <t>看起来</t>
-  </si>
-  <si>
-    <t>点</t>
-  </si>
-  <si>
-    <t>人生</t>
+    <t>好好</t>
   </si>
   <si>
     <t>越</t>
   </si>
   <si>
-    <t>世界</t>
-  </si>
-  <si>
-    <t>一下</t>
-  </si>
-  <si>
-    <t>特殊</t>
-  </si>
-  <si>
-    <t>不会</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>镜头</t>
-  </si>
-  <si>
-    <t>心情</t>
-  </si>
-  <si>
-    <t>标记</t>
-  </si>
-  <si>
-    <t>好好</t>
-  </si>
-  <si>
-    <t>年</t>
-  </si>
-  <si>
-    <t>吸引</t>
-  </si>
-  <si>
-    <t>内心</t>
-  </si>
-  <si>
-    <t>最近</t>
+    <t>感</t>
+  </si>
+  <si>
+    <t>之后</t>
+  </si>
+  <si>
+    <t>主角</t>
+  </si>
+  <si>
+    <t>看五叔</t>
+  </si>
+  <si>
+    <t>看看</t>
+  </si>
+  <si>
+    <t>总</t>
+  </si>
+  <si>
+    <t>下去</t>
   </si>
   <si>
     <t>两集</t>
   </si>
   <si>
-    <t>感</t>
+    <t>居然</t>
+  </si>
+  <si>
+    <t>有意思</t>
   </si>
   <si>
     <t>一定</t>
   </si>
   <si>
+    <t>韩国</t>
+  </si>
+  <si>
+    <t>最好</t>
+  </si>
+  <si>
+    <t>应该</t>
+  </si>
+  <si>
+    <t>起来</t>
+  </si>
+  <si>
+    <t>羡慕</t>
+  </si>
+  <si>
+    <t>简单</t>
+  </si>
+  <si>
     <t>第一集</t>
   </si>
   <si>
-    <t>主角</t>
-  </si>
-  <si>
-    <t>总</t>
-  </si>
-  <si>
-    <t>最好</t>
-  </si>
-  <si>
-    <t>应该</t>
-  </si>
-  <si>
-    <t>简单</t>
-  </si>
-  <si>
-    <t>韩国</t>
-  </si>
-  <si>
-    <t>起来</t>
-  </si>
-  <si>
-    <t>羡慕</t>
-  </si>
-  <si>
-    <t>有意思</t>
-  </si>
-  <si>
     <t>久</t>
   </si>
   <si>
-    <t>之后</t>
-  </si>
-  <si>
-    <t>下去</t>
-  </si>
-  <si>
-    <t>看五叔</t>
-  </si>
-  <si>
-    <t>居然</t>
+    <t>看过</t>
   </si>
   <si>
     <t>拍</t>
   </si>
   <si>
-    <t>看看</t>
-  </si>
-  <si>
-    <t>看过</t>
+    <t>北海道</t>
+  </si>
+  <si>
+    <t>啊啊啊</t>
+  </si>
+  <si>
+    <t>套路</t>
+  </si>
+  <si>
+    <t>少</t>
+  </si>
+  <si>
+    <t>海鲜</t>
+  </si>
+  <si>
+    <t>自由</t>
+  </si>
+  <si>
+    <t>不同</t>
+  </si>
+  <si>
+    <t>火锅</t>
+  </si>
+  <si>
+    <t>故事</t>
+  </si>
+  <si>
+    <t>依旧</t>
   </si>
   <si>
     <t>原来</t>
   </si>
   <si>
+    <t>快</t>
+  </si>
+  <si>
+    <t>非常</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>中国</t>
+  </si>
+  <si>
+    <t>烧</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>第五</t>
+  </si>
+  <si>
+    <t>身体</t>
+  </si>
+  <si>
+    <t>丰富</t>
+  </si>
+  <si>
     <t>感受</t>
   </si>
   <si>
-    <t>丰富</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>少</t>
+    <t>美味</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>炸</t>
+  </si>
+  <si>
+    <t>内心独白</t>
   </si>
   <si>
     <t>笑</t>
   </si>
   <si>
-    <t>非常</t>
-  </si>
-  <si>
-    <t>快</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>北海道</t>
-  </si>
-  <si>
-    <t>第五</t>
-  </si>
-  <si>
-    <t>美味</t>
-  </si>
-  <si>
-    <t>烧</t>
-  </si>
-  <si>
-    <t>海鲜</t>
-  </si>
-  <si>
-    <t>火锅</t>
-  </si>
-  <si>
-    <t>炸</t>
-  </si>
-  <si>
-    <t>依旧</t>
-  </si>
-  <si>
-    <t>内心独白</t>
-  </si>
-  <si>
-    <t>啊啊啊</t>
-  </si>
-  <si>
-    <t>套路</t>
-  </si>
-  <si>
-    <t>身体</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>中国</t>
-  </si>
-  <si>
-    <t>自由</t>
-  </si>
-  <si>
-    <t>故事</t>
-  </si>
-  <si>
-    <t>不同</t>
-  </si>
-  <si>
     <t>习惯</t>
   </si>
   <si>
+    <t>出差</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>评分</t>
+  </si>
+  <si>
+    <t>地方</t>
+  </si>
+  <si>
+    <t>期间</t>
+  </si>
+  <si>
+    <t>正餐</t>
+  </si>
+  <si>
+    <t>明年</t>
+  </si>
+  <si>
+    <t>下来</t>
+  </si>
+  <si>
+    <t>内容</t>
+  </si>
+  <si>
+    <t>一部</t>
+  </si>
+  <si>
+    <t>套餐</t>
+  </si>
+  <si>
+    <t>😋</t>
+  </si>
+  <si>
+    <t>事情</t>
+  </si>
+  <si>
+    <t>日式</t>
+  </si>
+  <si>
+    <t>日子</t>
+  </si>
+  <si>
+    <t>日剧</t>
+  </si>
+  <si>
+    <t>神奇</t>
+  </si>
+  <si>
+    <t>后面</t>
+  </si>
+  <si>
+    <t>饭菜</t>
+  </si>
+  <si>
+    <t>诱人</t>
+  </si>
+  <si>
+    <t>第十一</t>
+  </si>
+  <si>
+    <t>第一次</t>
+  </si>
+  <si>
+    <t>食堂</t>
+  </si>
+  <si>
+    <t>口味</t>
+  </si>
+  <si>
+    <t>第四集</t>
+  </si>
+  <si>
+    <t>台词</t>
+  </si>
+  <si>
+    <t>环节</t>
+  </si>
+  <si>
+    <t>努力</t>
+  </si>
+  <si>
+    <t>珍惜</t>
+  </si>
+  <si>
+    <t>选择</t>
+  </si>
+  <si>
+    <t>い</t>
+  </si>
+  <si>
+    <t>适合</t>
+  </si>
+  <si>
+    <t>干饭</t>
+  </si>
+  <si>
+    <t>追</t>
+  </si>
+  <si>
+    <t>竟然</t>
+  </si>
+  <si>
+    <t>电视剧</t>
+  </si>
+  <si>
+    <t>直接</t>
+  </si>
+  <si>
+    <t>第六</t>
+  </si>
+  <si>
+    <t>没想到</t>
+  </si>
+  <si>
+    <t>第二集</t>
+  </si>
+  <si>
+    <t>赛高</t>
+  </si>
+  <si>
+    <t>尝试</t>
+  </si>
+  <si>
+    <t>走</t>
+  </si>
+  <si>
     <t>老</t>
   </si>
   <si>
-    <t>😋</t>
-  </si>
-  <si>
-    <t>干饭</t>
-  </si>
-  <si>
-    <t>地方</t>
-  </si>
-  <si>
-    <t>神奇</t>
-  </si>
-  <si>
-    <t>下来</t>
+    <t>依然</t>
   </si>
   <si>
     <t>不知不觉</t>
   </si>
   <si>
-    <t>饭菜</t>
-  </si>
-  <si>
-    <t>第六</t>
-  </si>
-  <si>
-    <t>后面</t>
-  </si>
-  <si>
-    <t>尝试</t>
-  </si>
-  <si>
     <t>不能</t>
   </si>
   <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>第十一</t>
-  </si>
-  <si>
-    <t>竟然</t>
-  </si>
-  <si>
-    <t>套餐</t>
-  </si>
-  <si>
-    <t>一部</t>
-  </si>
-  <si>
-    <t>)</t>
-  </si>
-  <si>
-    <t>第四集</t>
-  </si>
-  <si>
-    <t>第一次</t>
+    <t>原作者</t>
   </si>
   <si>
     <t>第三季</t>
   </si>
   <si>
-    <t>第二集</t>
-  </si>
-  <si>
-    <t>内容</t>
-  </si>
-  <si>
-    <t>评分</t>
-  </si>
-  <si>
-    <t>走</t>
-  </si>
-  <si>
-    <t>正餐</t>
-  </si>
-  <si>
-    <t>日式</t>
-  </si>
-  <si>
-    <t>明年</t>
-  </si>
-  <si>
-    <t>日剧</t>
-  </si>
-  <si>
-    <t>依然</t>
-  </si>
-  <si>
-    <t>事情</t>
-  </si>
-  <si>
-    <t>努力</t>
-  </si>
-  <si>
-    <t>出差</t>
-  </si>
-  <si>
-    <t>环节</t>
-  </si>
-  <si>
-    <t>没想到</t>
-  </si>
-  <si>
-    <t>期间</t>
-  </si>
-  <si>
-    <t>原作者</t>
-  </si>
-  <si>
-    <t>珍惜</t>
-  </si>
-  <si>
-    <t>赛高</t>
-  </si>
-  <si>
-    <t>电视剧</t>
-  </si>
-  <si>
-    <t>日子</t>
-  </si>
-  <si>
-    <t>适合</t>
-  </si>
-  <si>
-    <t>台词</t>
-  </si>
-  <si>
-    <t>选择</t>
-  </si>
-  <si>
-    <t>直接</t>
-  </si>
-  <si>
     <t>开</t>
   </si>
   <si>
-    <t>口味</t>
-  </si>
-  <si>
-    <t>食堂</t>
-  </si>
-  <si>
-    <t>诱人</t>
-  </si>
-  <si>
-    <t>追</t>
-  </si>
-  <si>
-    <t>い</t>
+    <t>中华</t>
+  </si>
+  <si>
+    <t>真实</t>
+  </si>
+  <si>
+    <t>今年</t>
+  </si>
+  <si>
+    <t>番</t>
+  </si>
+  <si>
+    <t>减肥</t>
+  </si>
+  <si>
+    <t>白吃</t>
+  </si>
+  <si>
+    <t>内脏</t>
+  </si>
+  <si>
+    <t>煎</t>
+  </si>
+  <si>
+    <t>活动</t>
+  </si>
+  <si>
+    <t>不可</t>
+  </si>
+  <si>
+    <t>肚子</t>
   </si>
   <si>
     <t>不用</t>
   </si>
   <si>
-    <t>不可</t>
-  </si>
-  <si>
-    <t>(</t>
+    <t>美好</t>
   </si>
   <si>
     <t>羊肉</t>
   </si>
   <si>
+    <t>突然</t>
+  </si>
+  <si>
+    <t>买</t>
+  </si>
+  <si>
+    <t>节奏</t>
+  </si>
+  <si>
+    <t>纠结</t>
+  </si>
+  <si>
+    <t>牛舌</t>
+  </si>
+  <si>
+    <t>会员</t>
+  </si>
+  <si>
+    <t>米饭</t>
+  </si>
+  <si>
+    <t>算是</t>
+  </si>
+  <si>
+    <t>牛肉</t>
+  </si>
+  <si>
+    <t>真正</t>
+  </si>
+  <si>
+    <t>变得</t>
+  </si>
+  <si>
+    <t>🥰</t>
+  </si>
+  <si>
+    <t>部分</t>
+  </si>
+  <si>
+    <t>面</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>鱼</t>
+  </si>
+  <si>
+    <t>一家</t>
+  </si>
+  <si>
+    <t>さ</t>
+  </si>
+  <si>
+    <t>呜呜</t>
+  </si>
+  <si>
+    <t>饭量</t>
+  </si>
+  <si>
+    <t>搞笑</t>
+  </si>
+  <si>
+    <t>过程</t>
+  </si>
+  <si>
+    <t>一点</t>
+  </si>
+  <si>
+    <t>想起</t>
+  </si>
+  <si>
+    <t>饭前</t>
+  </si>
+  <si>
+    <t>餐馆</t>
+  </si>
+  <si>
+    <t>超级</t>
+  </si>
+  <si>
+    <t>客户</t>
+  </si>
+  <si>
+    <t>实在</t>
+  </si>
+  <si>
+    <t>咚咚</t>
+  </si>
+  <si>
+    <t>战歌</t>
+  </si>
+  <si>
+    <t>轻松</t>
+  </si>
+  <si>
+    <t>加</t>
+  </si>
+  <si>
+    <t>慢慢</t>
+  </si>
+  <si>
     <t>最想</t>
   </si>
   <si>
-    <t>🥰</t>
-  </si>
-  <si>
-    <t>美好</t>
-  </si>
-  <si>
-    <t>活动</t>
+    <t>补</t>
+  </si>
+  <si>
+    <t>可能</t>
   </si>
   <si>
     <t>回来</t>
-  </si>
-  <si>
-    <t>减肥</t>
-  </si>
-  <si>
-    <t>内脏</t>
-  </si>
-  <si>
-    <t>纠结</t>
-  </si>
-  <si>
-    <t>节奏</t>
-  </si>
-  <si>
-    <t>肚子</t>
-  </si>
-  <si>
-    <t>真实</t>
-  </si>
-  <si>
-    <t>牛舌</t>
-  </si>
-  <si>
-    <t>米饭</t>
-  </si>
-  <si>
-    <t>算是</t>
-  </si>
-  <si>
-    <t>买</t>
-  </si>
-  <si>
-    <t>真正</t>
-  </si>
-  <si>
-    <t>可能</t>
-  </si>
-  <si>
-    <t>当时</t>
-  </si>
-  <si>
-    <t>突然</t>
-  </si>
-  <si>
-    <t>变得</t>
-  </si>
-  <si>
-    <t>白吃</t>
-  </si>
-  <si>
-    <t>番</t>
-  </si>
-  <si>
-    <t>想起</t>
-  </si>
-  <si>
-    <t>今年</t>
-  </si>
-  <si>
-    <t>慢慢</t>
-  </si>
-  <si>
-    <t>战歌</t>
-  </si>
-  <si>
-    <t>呜呜</t>
-  </si>
-  <si>
-    <t>搞笑</t>
-  </si>
-  <si>
-    <t>客户</t>
-  </si>
-  <si>
-    <t>会员</t>
-  </si>
-  <si>
-    <t>咚咚</t>
-  </si>
-  <si>
-    <t>中华</t>
-  </si>
-  <si>
-    <t>加</t>
-  </si>
-  <si>
-    <t>实在</t>
-  </si>
-  <si>
-    <t>煎</t>
-  </si>
-  <si>
-    <t>11</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>209</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1313,7 +1313,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>165</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1321,7 +1321,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>152</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1329,7 +1329,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1337,7 +1337,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1345,7 +1345,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1353,7 +1353,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1361,7 +1361,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1369,7 +1369,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1377,7 +1377,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1385,7 +1385,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1393,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1401,7 +1401,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1409,7 +1409,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1417,7 +1417,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1425,7 +1425,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1433,7 +1433,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1441,7 +1441,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1457,7 +1457,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1465,7 +1465,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1473,7 +1473,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1481,7 +1481,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1489,7 +1489,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1497,7 +1497,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1505,7 +1505,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1513,7 +1513,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1521,7 +1521,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1529,7 +1529,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1537,7 +1537,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1545,7 +1545,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1553,7 +1553,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1561,7 +1561,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1569,7 +1569,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1577,7 +1577,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1585,7 +1585,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1593,7 +1593,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1601,7 +1601,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1609,7 +1609,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1617,7 +1617,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1625,7 +1625,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1633,7 +1633,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1641,7 +1641,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1649,7 +1649,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1657,7 +1657,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1665,7 +1665,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1673,7 +1673,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1681,7 +1681,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1689,7 +1689,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1697,7 +1697,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1705,7 +1705,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1713,7 +1713,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1721,7 +1721,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1729,7 +1729,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1745,7 +1745,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1753,7 +1753,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1761,7 +1761,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1769,7 +1769,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1777,7 +1777,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1785,7 +1785,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1793,7 +1793,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1801,7 +1801,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1809,7 +1809,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1817,7 +1817,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1825,7 +1825,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1833,7 +1833,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1841,7 +1841,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1849,7 +1849,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1857,7 +1857,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1865,7 +1865,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1873,7 +1873,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1881,7 +1881,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1889,7 +1889,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1897,7 +1897,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1905,7 +1905,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1913,7 +1913,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1921,7 +1921,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1929,7 +1929,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1937,7 +1937,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1945,7 +1945,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1953,7 +1953,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1961,7 +1961,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1969,7 +1969,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1977,7 +1977,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1985,7 +1985,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1993,7 +1993,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2001,7 +2001,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2009,7 +2009,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2017,7 +2017,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2025,7 +2025,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2033,7 +2033,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2041,7 +2041,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2049,7 +2049,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2057,7 +2057,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2065,7 +2065,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2073,7 +2073,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2081,7 +2081,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2089,7 +2089,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2097,7 +2097,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2105,7 +2105,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2113,7 +2113,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2145,7 +2145,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2153,7 +2153,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2161,7 +2161,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2169,7 +2169,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2177,7 +2177,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2185,7 +2185,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2193,7 +2193,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2201,7 +2201,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2209,7 +2209,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2217,7 +2217,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2225,7 +2225,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2233,7 +2233,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2241,7 +2241,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2249,7 +2249,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2257,7 +2257,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2265,7 +2265,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2273,7 +2273,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2281,7 +2281,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2289,7 +2289,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2297,7 +2297,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2305,7 +2305,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2313,7 +2313,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2353,7 +2353,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2361,7 +2361,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2369,7 +2369,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2377,7 +2377,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2385,7 +2385,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2393,7 +2393,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2401,7 +2401,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2409,7 +2409,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2417,7 +2417,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2425,7 +2425,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2433,7 +2433,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2497,7 +2497,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2505,7 +2505,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2513,7 +2513,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2521,7 +2521,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2529,7 +2529,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2537,7 +2537,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2545,7 +2545,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2553,7 +2553,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2561,7 +2561,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2569,7 +2569,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2577,7 +2577,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2665,7 +2665,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2673,7 +2673,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2681,7 +2681,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2689,7 +2689,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2697,7 +2697,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2705,7 +2705,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2713,7 +2713,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2721,7 +2721,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2729,7 +2729,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2737,7 +2737,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2745,7 +2745,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2873,7 +2873,7 @@
         <v>199</v>
       </c>
       <c r="B199">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2881,7 +2881,7 @@
         <v>200</v>
       </c>
       <c r="B200">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2889,7 +2889,7 @@
         <v>201</v>
       </c>
       <c r="B201">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2897,7 +2897,7 @@
         <v>202</v>
       </c>
       <c r="B202">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2905,7 +2905,7 @@
         <v>203</v>
       </c>
       <c r="B203">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2913,7 +2913,7 @@
         <v>204</v>
       </c>
       <c r="B204">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2921,7 +2921,7 @@
         <v>205</v>
       </c>
       <c r="B205">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2929,7 +2929,7 @@
         <v>206</v>
       </c>
       <c r="B206">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2937,7 +2937,7 @@
         <v>207</v>
       </c>
       <c r="B207">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2945,7 +2945,7 @@
         <v>208</v>
       </c>
       <c r="B208">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2953,7 +2953,7 @@
         <v>209</v>
       </c>
       <c r="B209">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -3281,7 +3281,7 @@
         <v>250</v>
       </c>
       <c r="B250">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -3289,7 +3289,7 @@
         <v>251</v>
       </c>
       <c r="B251">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -3297,7 +3297,7 @@
         <v>252</v>
       </c>
       <c r="B252">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -3305,7 +3305,7 @@
         <v>253</v>
       </c>
       <c r="B253">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -3313,7 +3313,7 @@
         <v>254</v>
       </c>
       <c r="B254">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -3321,7 +3321,7 @@
         <v>255</v>
       </c>
       <c r="B255">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -3329,7 +3329,7 @@
         <v>256</v>
       </c>
       <c r="B256">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -3337,7 +3337,7 @@
         <v>257</v>
       </c>
       <c r="B257">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -3345,7 +3345,7 @@
         <v>258</v>
       </c>
       <c r="B258">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -3353,7 +3353,7 @@
         <v>259</v>
       </c>
       <c r="B259">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -3361,7 +3361,7 @@
         <v>260</v>
       </c>
       <c r="B260">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -3369,7 +3369,7 @@
         <v>261</v>
       </c>
       <c r="B261">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="262" spans="1:2">

</xml_diff>